<commit_message>
Subindo site institucional rodando em node
</commit_message>
<xml_diff>
--- a/Documentação/Excel/ControleExecução.xlsx
+++ b/Documentação/Excel/ControleExecução.xlsx
@@ -5,20 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betis\Documents\FACULDADEAES\Semestre2\Procastinator\Grupo-1-adsa\Documentação\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betis\Documents\FACULDADEADS\Semestre2\Procastinator\Grupo-1-adsa\Documentação\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EF63C2-6793-4F95-A81D-980BE249337C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFB1558-38C1-48C8-8572-179B37C54F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C6CCD9A-559E-4466-B2B6-8A9365E6E347}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{3C6CCD9A-559E-4466-B2B6-8A9365E6E347}"/>
   </bookViews>
   <sheets>
-    <sheet name="Atividades" sheetId="1" r:id="rId1"/>
-    <sheet name="Contador" sheetId="2" r:id="rId2"/>
+    <sheet name="Semana 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Semana 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Semana 3" sheetId="5" r:id="rId3"/>
+    <sheet name="Semana 4" sheetId="1" r:id="rId4"/>
+    <sheet name="Contador" sheetId="2" r:id="rId5"/>
+    <sheet name="Planilha1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="61">
   <si>
     <t>Atividades</t>
   </si>
@@ -188,13 +192,46 @@
   </si>
   <si>
     <t>Datas finalizar</t>
+  </si>
+  <si>
+    <t>Coluna2</t>
+  </si>
+  <si>
+    <t>Breno</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Ellen</t>
+  </si>
+  <si>
+    <t>Ellen e Leu</t>
+  </si>
+  <si>
+    <t>Beatriz e Julio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe no código </t>
+  </si>
+  <si>
+    <t>Fe na VM</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Beatriz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beatriz e Fernando </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,21 +263,13 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,18 +320,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -310,6 +327,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -442,29 +483,40 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="30">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -663,6 +715,534 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -684,7 +1264,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Beatriz Nascimento" refreshedDate="44482.837558333333" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="23" xr:uid="{8D1FB19E-6D73-4955-9CAA-ADE811379436}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Beatriz Nascimento" refreshedDate="44484.789923958335" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="23" xr:uid="{8D1FB19E-6D73-4955-9CAA-ADE811379436}">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela1"/>
   </cacheSource>
@@ -734,7 +1314,7 @@
     <s v="JAR inicial rodando em Cliente Linux em VM: Sistemas Op"/>
     <x v="2"/>
     <s v="Grupo individual"/>
-    <m/>
+    <s v="Sábado"/>
   </r>
   <r>
     <s v="Inovação"/>
@@ -767,22 +1347,22 @@
     <s v="Sábado"/>
   </r>
   <r>
-    <s v="Controle da Execução"/>
-    <x v="2"/>
-    <s v="Bia e Breno"/>
-    <m/>
-  </r>
-  <r>
     <s v="Jar Inicial Console conectado no Banco: Ling. Programação"/>
     <x v="2"/>
     <s v="Fernando e Julio"/>
-    <m/>
+    <s v="Sábado"/>
   </r>
   <r>
     <s v="API email com nodemailer"/>
     <x v="2"/>
     <s v="Bia e Julio"/>
-    <m/>
+    <s v="Sábado"/>
+  </r>
+  <r>
+    <s v="Controle da Execução"/>
+    <x v="3"/>
+    <s v="Grupo"/>
+    <s v="ok"/>
   </r>
   <r>
     <s v="Protótipo Funcional do Java: Ling. Programação"/>
@@ -919,13 +1499,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A36552AB-2795-429B-88D4-9C89CD5A67D5}" name="Tabela1" displayName="Tabela1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D24" xr:uid="{A36552AB-2795-429B-88D4-9C89CD5A67D5}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{66B46BE1-2315-4D69-90BE-E4B6CC8C5D83}" name="Atividades" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{173CAD7C-3C09-4100-9643-07470DDE0823}" name="Status" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{78D39DDD-0E3C-42BF-A3EC-61A94CF34A2E}" name="Coluna1" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{E4D9AEA7-B0BF-4705-BC56-0259A0775324}" name="Datas finalizar" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{723C81B2-B040-4447-A283-444B76DD325A}" name="Tabela13" displayName="Tabela13" ref="A1:C24" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A1:C24" xr:uid="{723C81B2-B040-4447-A283-444B76DD325A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1436B39E-1590-4D1A-BACF-DF9A55D18051}" name="Atividades" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{0567A1FD-B8F2-4F0E-BEC1-C0CA9C4D7DD4}" name="Status" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{D093FBA9-F896-47F0-87D0-DD885B37CB86}" name="Coluna1" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{673FF606-EE4F-4783-9982-58AE77A64F18}" name="Tabela14" displayName="Tabela14" ref="A1:C24" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+  <autoFilter ref="A1:C24" xr:uid="{673FF606-EE4F-4783-9982-58AE77A64F18}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{18D7CC45-70D9-484E-BFEA-F7D143CEF19E}" name="Atividades" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{95EFDDBA-4AEC-41AC-835F-4D3C820508DC}" name="Status" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{65B40D47-4DAE-4D13-9595-D5590BB9659B}" name="Coluna1" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D0284512-E713-4742-A255-9D6E1A10D397}" name="Tabela145" displayName="Tabela145" ref="A1:C24" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:C24" xr:uid="{D0284512-E713-4742-A255-9D6E1A10D397}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BA5B91CC-6D12-4397-84E6-E21C250CDFE7}" name="Atividades" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{12790145-663C-42F7-B07F-3BBAC238DA06}" name="Status" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{17ADF25A-72A5-4997-A49E-92F08FE84FA4}" name="Coluna1" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A36552AB-2795-429B-88D4-9C89CD5A67D5}" name="Tabela1" displayName="Tabela1" ref="A1:E24" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E24" xr:uid="{A36552AB-2795-429B-88D4-9C89CD5A67D5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{66B46BE1-2315-4D69-90BE-E4B6CC8C5D83}" name="Atividades" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{173CAD7C-3C09-4100-9643-07470DDE0823}" name="Status" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{78D39DDD-0E3C-42BF-A3EC-61A94CF34A2E}" name="Coluna1" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{E4D9AEA7-B0BF-4705-BC56-0259A0775324}" name="Datas finalizar" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C1C42D66-7E8C-4069-8027-D5A2BAC43CD2}" name="Coluna2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1227,22 +1844,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC07DF6-994F-47BE-9010-28DB6A8FF7C6}">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403CBFAE-542E-4851-BF99-7BB323815EE4}">
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1252,329 +1868,261 @@
       <c r="C1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="12" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="20" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="17" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="24"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="24"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1583,11 +2131,961 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA192A7-8C16-4085-9098-4775E7C5487D}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A12242-E909-4F31-874F-7CAECA6B729A}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC07DF6-994F-47BE-9010-28DB6A8FF7C6}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="28"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FDA779-461B-41B4-8767-EC4F97E12650}">
   <dimension ref="A3:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +3123,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1633,7 +3131,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1650,6 +3148,79 @@
       </c>
       <c r="B9" s="3">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A2CD804-3964-40C8-B3C5-F4333DDF7B29}">
+  <dimension ref="A3:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subindo controle de execução
</commit_message>
<xml_diff>
--- a/Documentação/Excel/ControleExecução.xlsx
+++ b/Documentação/Excel/ControleExecução.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betis\Documents\FACULDADEADS\Semestre2\Procastinator\Grupo-1-adsa\Documentação\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD4C0A2-8C6F-4AF9-B347-EE0C4DBFC94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD7C5B8-1412-46CE-AD96-DBE076DF42AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3C6CCD9A-559E-4466-B2B6-8A9365E6E347}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="61">
   <si>
     <t>Atividades</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t xml:space="preserve">Beatriz e Fernando </t>
+  </si>
+  <si>
+    <t>Terceiro semestre</t>
   </si>
 </sst>
 </file>
@@ -2697,7 +2700,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3038,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D24" s="28"/>
     </row>

</xml_diff>